<commit_message>
classification items fixed and upload script adapted to new structure.
</commit_message>
<xml_diff>
--- a/mySQL_Create/classification_items.xlsx
+++ b/mySQL_Create/classification_items.xlsx
@@ -626,7 +626,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +773,7 @@
         <v>38</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>20</v>

</xml_diff>